<commit_message>
test(fix): force timezone to consistently be UTC
</commit_message>
<xml_diff>
--- a/cmd/excalibur/testdata/output_expected.xlsx
+++ b/cmd/excalibur/testdata/output_expected.xlsx
@@ -1227,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="32">
-        <v>45306.395833333336</v>
+        <v>45306.354166666664</v>
       </c>
       <c r="E15" s="33">
         <v>46022</v>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="34">
-        <v>45231.666666666664</v>
+        <v>45231.625</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="15" t="s">

</xml_diff>